<commit_message>
Allow import of formula-based answers
Some questionnaires (SVRS98) use simple formula for answers. We now allow
them to be imported as hardcoded values (formula is lost). Also we do not
import null values anymore.
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="942" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="469" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables_W" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
   <si>
     <t>Survey Category</t>
   </si>
@@ -100,6 +100,9 @@
     <t>Cat 2-5</t>
   </si>
   <si>
+    <t>formula with alternate category will also be imported</t>
+  </si>
+  <si>
     <t>Cat 2-6</t>
   </si>
   <si>
@@ -325,9 +328,6 @@
     <t>B Cat 1-5</t>
   </si>
   <si>
-    <t>Alternate B Category 2</t>
-  </si>
-  <si>
     <t>B Category 2</t>
   </si>
   <si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>B Cat 2-10</t>
+  </si>
+  <si>
+    <t>Alternate B Category 3</t>
   </si>
   <si>
     <t>B Category 3</t>
@@ -611,7 +614,10 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -631,14 +637,15 @@
   </sheetPr>
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F11" activeCellId="0" pane="topLeft" sqref="F11"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3058823529412"/>
-    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="15.2235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3010204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.6887755102041"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -839,15 +846,15 @@
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
-        <v>50.4</v>
+        <v>66.4</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",E12:E53)=0,"",SUMIF(A12:A53,"&gt;""",E12:E53))</f>
-        <v>91.3</v>
+        <v>94.3</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",F12:F53)=0,"",SUMIF(A12:A53,"&gt;""",F12:F53))</f>
-        <v>74.6</v>
+        <v>82.6</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>19</v>
@@ -871,15 +878,15 @@
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",E14:E17)+SUMIF(A26:A29,"&gt;""",E26:E29)+SUMIF(A46:A49,"&gt;""",E46:E49)+SUMIF(A34:A37,"&gt;""",E34:E37)=0,"",SUMIF(A14:A17,"&gt;""",E14:E17)+SUMIF(A26:A29,"&gt;""",E26:E29)+SUMIF(A46:A49,"&gt;""",E46:E49)+SUMIF(A34:A37,"&gt;""",E34:E37))</f>
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",F14:F17)+SUMIF(A26:A29,"&gt;""",F26:F29)+SUMIF(A46:A49,"&gt;""",F46:F49)+SUMIF(A34:A37,"&gt;""",F34:F37)=0,"",SUMIF(A14:A17,"&gt;""",F14:F17)+SUMIF(A26:A29,"&gt;""",F26:F29)+SUMIF(A46:A49,"&gt;""",F46:F49)+SUMIF(A34:A37,"&gt;""",F34:F37))</f>
-        <v>66.6</v>
+        <v>74.6</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>20</v>
@@ -1026,23 +1033,26 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
+      <c r="A17" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="C17" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="0" t="str">
-        <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D37),ISNUMBER(D49)),SUM(D29,D37,D49),"")</f>
-        <v/>
-      </c>
-      <c r="E17" s="0" t="str">
-        <f aca="false">IF(OR(ISNUMBER(E29),ISNUMBER(E37),ISNUMBER(E49)),SUM(E29,E37,E49),"")</f>
-        <v/>
-      </c>
-      <c r="F17" s="0" t="str">
-        <f aca="false">IF(OR(ISNUMBER(F29),ISNUMBER(F37),ISNUMBER(F49)),SUM(F29,F37,F49),"")</f>
-        <v/>
+        <v>26</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">4*4</f>
+        <v>16</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <f aca="false">2+1</f>
+        <v>3</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <f aca="false">3+5</f>
+        <v>8</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J29),ISNUMBER(J37),ISNUMBER(J49)),SUM(J29,J37,J49),"")</f>
@@ -1059,7 +1069,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -1074,7 +1084,7 @@
         <v/>
       </c>
       <c r="I18" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G38),ISTEXT(G50)),SUM(J38,J50),IF(OR(ISNUMBER(J19),ISNUMBER(J20),ISNUMBER(J21)),SUM(J19,J20,J21),""))</f>
@@ -1091,7 +1101,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -1106,7 +1116,7 @@
         <v/>
       </c>
       <c r="I19" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J39),ISNUMBER(J51)),SUM(J39,J51),"")</f>
@@ -1123,7 +1133,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -1138,7 +1148,7 @@
         <v/>
       </c>
       <c r="I20" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J40),ISNUMBER(J52)),SUM(J40,J52),"")</f>
@@ -1155,7 +1165,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -1170,7 +1180,7 @@
         <v/>
       </c>
       <c r="I21" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J41),ISNUMBER(J53)),SUM(J41,J53),"")</f>
@@ -1187,10 +1197,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="B22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J22" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J23),ISNUMBER(J24),ISNUMBER(J25),ISNUMBER(J26),ISNUMBER(J27),ISNUMBER(J28),ISNUMBER(J29),ISNUMBER(J30),ISNUMBER(J31),ISNUMBER(J32),ISNUMBER(J33),ISNUMBER(J34),ISNUMBER(J35),ISNUMBER(J36),ISNUMBER(J37),ISNUMBER(J38),ISNUMBER(J39),ISNUMBER(J40),ISNUMBER(J41)),SUMIF(G23:G41,"&gt;""",J23:J41),"")</f>
@@ -1207,7 +1217,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -1222,7 +1232,7 @@
         <v/>
       </c>
       <c r="I23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J27),ISNUMBER(J31)),SUM(J27,J31),"")</f>
@@ -1239,7 +1249,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -1254,7 +1264,7 @@
         <v/>
       </c>
       <c r="I24" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J28),ISNUMBER(J32)),SUM(J28,J32),"")</f>
@@ -1271,7 +1281,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -1286,7 +1296,7 @@
         <v/>
       </c>
       <c r="I25" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J29),ISNUMBER(J33)),SUM(J29,J33),"")</f>
@@ -1303,10 +1313,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -1318,10 +1328,10 @@
         <v>66.6</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>22</v>
@@ -1335,34 +1345,34 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -1374,10 +1384,10 @@
         <v>8</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>1</v>
@@ -1391,7 +1401,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -1406,7 +1416,7 @@
         <v/>
       </c>
       <c r="I31" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J35),ISNUMBER(J39)),SUM(J35,J39),"")</f>
@@ -1423,7 +1433,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -1438,7 +1448,7 @@
         <v/>
       </c>
       <c r="I32" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J36),ISNUMBER(J40)),SUM(J36,J40),"")</f>
@@ -1455,7 +1465,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -1470,7 +1480,7 @@
         <v/>
       </c>
       <c r="I33" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J37),ISNUMBER(J41)),SUM(J37,J41),"")</f>
@@ -1487,7 +1497,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -1502,7 +1512,7 @@
         <v/>
       </c>
       <c r="I34" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G35),ISTEXT(G36),ISTEXT(G37)),SUM(J35,J36,J37),"")</f>
@@ -1519,31 +1529,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -1558,7 +1568,7 @@
         <v/>
       </c>
       <c r="I38" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G39),ISTEXT(G40),ISTEXT(G41)),SUM(J39,J40,J41),"")</f>
@@ -1575,31 +1585,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -1614,7 +1624,7 @@
         <v/>
       </c>
       <c r="I42" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J43),ISNUMBER(J44),ISNUMBER(J45),ISNUMBER(J46),ISNUMBER(J47),ISNUMBER(J48),ISNUMBER(J49),ISNUMBER(J50),ISNUMBER(J51),ISNUMBER(J52),ISNUMBER(J53)),SUMIF(G43:G53,"&gt;""",J43:J53),"")</f>
@@ -1631,7 +1641,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -1646,7 +1656,7 @@
         <v/>
       </c>
       <c r="I43" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J47),ISNUMBER(J51)),SUM(J47,J51),"")</f>
@@ -1663,7 +1673,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -1678,7 +1688,7 @@
         <v/>
       </c>
       <c r="H44" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J48),ISNUMBER(J52)),SUM(J48,J52),"")</f>
@@ -1695,7 +1705,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -1706,7 +1716,7 @@
         <v/>
       </c>
       <c r="I45" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(K49),ISNUMBER(K53)),SUM(K49,K53),"")</f>
@@ -1719,7 +1729,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -1734,7 +1744,7 @@
         <v/>
       </c>
       <c r="I46" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G47),ISTEXT(G48),ISTEXT(G49)),SUM(J47,J48,J49),"")</f>
@@ -1751,31 +1761,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -1790,7 +1800,7 @@
         <v/>
       </c>
       <c r="I50" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G51),ISTEXT(G52),ISTEXT(G53)),SUM(J51,J52,J53),"")</f>
@@ -1807,31 +1817,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -1846,7 +1856,7 @@
         <v/>
       </c>
       <c r="I54" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J55),ISNUMBER(J56)),SUM(J55,J56),"")</f>
@@ -1863,23 +1873,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -1894,7 +1904,7 @@
         <v/>
       </c>
       <c r="I57" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J58),ISNUMBER(J59)),SUM(J58,J59),"")</f>
@@ -1911,23 +1921,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -1942,7 +1952,7 @@
         <v>9.8</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J60" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J61),ISNUMBER(J62),ISNUMBER(J63),ISNUMBER(J64),ISNUMBER(J65),ISNUMBER(J66),ISNUMBER(J67)),SUM(J61:J67),"")</f>
@@ -1959,10 +1969,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -1974,31 +1984,31 @@
         <v>7</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -2010,36 +2020,36 @@
         <v>2.8</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -2054,7 +2064,7 @@
         <v/>
       </c>
       <c r="I68" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J69),ISNUMBER(J70)),SUM(J69,J70),"")</f>
@@ -2071,23 +2081,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -2102,7 +2112,7 @@
         <v>0.1</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J72),ISNUMBER(J73),ISNUMBER(J74),ISNUMBER(J75)),SUM(J72:J75),"")</f>
@@ -2119,23 +2129,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -2147,7 +2157,7 @@
         <v>0.1</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J74" s="0" t="n">
         <v>5</v>
@@ -2161,15 +2171,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -2181,7 +2191,7 @@
         <v>0.1</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="77">
@@ -2190,15 +2200,15 @@
       </c>
       <c r="D77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D5),ISNUMBER(D11),ISNUMBER(D54),ISNUMBER(D57),ISNUMBER(D60),ISNUMBER(D71),ISNUMBER(D76)),SUM(D5,D11,D54,D57,D60,D68,D71,D76),"")</f>
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="E77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(E5),ISNUMBER(E11),ISNUMBER(E54),ISNUMBER(E57),ISNUMBER(E60),ISNUMBER(E71),ISNUMBER(E76)),SUM(E5,E11,E54,E57,E60,E68,E71,E76),"")</f>
-        <v>98.9</v>
+        <v>101.9</v>
       </c>
       <c r="F77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(F5),ISNUMBER(F11),ISNUMBER(F54),ISNUMBER(F57),ISNUMBER(F60),ISNUMBER(F71),ISNUMBER(F76)),SUM(F5,F11,F54,F57,F60,F68,F71,F76),"")</f>
-        <v>91.2</v>
+        <v>99.2</v>
       </c>
       <c r="H77" s="0" t="s">
         <v>10</v>
@@ -2234,22 +2244,23 @@
   </sheetPr>
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="1" pane="topLeft" sqref="G1 A2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A22" activeCellId="0" pane="topLeft" sqref="A22"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3058823529412"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="15.2235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.6887755102041"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>2</v>
@@ -2257,7 +2268,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
@@ -2270,7 +2281,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>8</v>
@@ -2284,7 +2295,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -2301,7 +2312,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -2318,10 +2329,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -2335,15 +2346,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -2357,13 +2368,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
-      <c r="A11" s="0" t="s">
-        <v>100</v>
-      </c>
       <c r="B11" s="0" t="s">
         <v>101</v>
       </c>
@@ -2554,13 +2562,16 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
+      <c r="A22" s="0" t="s">
+        <v>113</v>
+      </c>
       <c r="B22" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -2577,7 +2588,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -2594,7 +2605,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -2611,10 +2622,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -2628,25 +2639,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -2660,7 +2671,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -2677,7 +2688,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -2694,7 +2705,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -2711,7 +2722,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -2728,22 +2739,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -2760,22 +2771,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -2792,7 +2803,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -2809,7 +2820,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -2826,7 +2837,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -2839,7 +2850,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -2856,22 +2867,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -2888,22 +2899,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -2920,17 +2931,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -2947,17 +2958,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -2974,10 +2985,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -2991,17 +3002,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -3015,22 +3026,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -3047,17 +3058,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -3074,17 +3085,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -3098,12 +3109,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Import exclude rules from Excel files
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="469" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="940" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables_W" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="177">
   <si>
     <t>Survey Category</t>
   </si>
@@ -290,6 +290,21 @@
   </si>
   <si>
     <t>Cat 4-32</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Foo</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t>B Survey Category</t>
@@ -545,8 +560,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="165"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -613,8 +629,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -635,10 +655,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L77"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F11" activeCellId="0" pane="topLeft" sqref="F11"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A70" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A93" activeCellId="0" pane="topLeft" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2224,6 +2244,43 @@
       <c r="L77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(L5),ISNUMBER(L11),ISNUMBER(L54),ISNUMBER(L57),ISNUMBER(L60),ISNUMBER(L71),ISNUMBER(L76)),SUM(L5,L11,L54,L57,L60,L68,L71,L76),"")</f>
         <v>70</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="91">
+      <c r="D91" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="92">
+      <c r="D92" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="93">
+      <c r="D93" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" s="0" t="str">
+        <f aca="false">IF(F91="Foo", "No")</f>
+        <v>No</v>
+      </c>
+      <c r="J93" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="K93" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2242,10 +2299,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A22" activeCellId="0" pane="topLeft" sqref="A22"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A68" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D99" activeCellId="0" pane="topLeft" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2257,10 +2314,10 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>2</v>
@@ -2268,7 +2325,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
@@ -2281,7 +2338,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>8</v>
@@ -2295,7 +2352,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -2312,7 +2369,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -2329,10 +2386,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -2346,15 +2403,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -2368,12 +2425,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
@@ -2390,7 +2447,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
@@ -2407,7 +2464,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -2424,10 +2481,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -2444,7 +2501,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -2461,7 +2518,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
@@ -2478,7 +2535,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="C17" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D37),ISNUMBER(D49)),SUM(D29,D37,D49),"")</f>
@@ -2495,7 +2552,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -2512,7 +2569,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -2529,7 +2586,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -2546,7 +2603,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -2563,15 +2620,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -2588,7 +2645,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -2605,7 +2662,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -2622,10 +2679,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -2639,25 +2696,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -2671,7 +2728,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -2688,7 +2745,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -2705,7 +2762,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -2722,7 +2779,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -2739,22 +2796,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -2771,22 +2828,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -2803,7 +2860,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -2820,7 +2877,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -2837,7 +2894,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -2850,7 +2907,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -2867,22 +2924,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -2899,22 +2956,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -2931,17 +2988,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -2958,17 +3015,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -2985,10 +3042,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -3002,17 +3059,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -3026,22 +3083,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -3058,17 +3115,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -3085,17 +3142,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -3109,12 +3166,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -3141,6 +3198,32 @@
       <c r="F77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(F5),ISNUMBER(F11),ISNUMBER(F54),ISNUMBER(F57),ISNUMBER(F60),ISNUMBER(F71),ISNUMBER(F76)),SUM(F5,F11,F54,F57,F60,F68,F71,F76),"")</f>
         <v>157.8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="96">
+      <c r="D96" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="97">
+      <c r="E97" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="98">
+      <c r="F98" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="99">
+      <c r="D99" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F99" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unit test that questionnaires are not imported twice (but existing one are loaded from DB)
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="176">
   <si>
     <t>Survey Category</t>
   </si>
@@ -308,9 +308,6 @@
   </si>
   <si>
     <t>B Survey Category</t>
-  </si>
-  <si>
-    <t>Code 3</t>
   </si>
   <si>
     <t>Survey name 3 B</t>
@@ -562,7 +559,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="165"/>
+    <numFmt formatCode="GENERAL" numFmtId="165"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -657,11 +654,11 @@
   </sheetPr>
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A70" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A93" activeCellId="0" pane="topLeft" sqref="A93"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D3" activeCellId="0" pane="topLeft" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3010204081633"/>
     <col collapsed="false" hidden="false" max="12" min="2" style="0" width="15.2295918367347"/>
@@ -2257,7 +2254,7 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="92">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="D92" s="0" t="s">
         <v>92</v>
       </c>
@@ -2265,11 +2262,13 @@
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="93">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
       <c r="D93" s="1" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E93" s="1" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F93" s="0" t="str">
@@ -2301,8 +2300,8 @@
   </sheetPr>
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A68" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D99" activeCellId="0" pane="topLeft" sqref="D99"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D4" activeCellId="0" pane="topLeft" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2317,7 +2316,7 @@
         <v>94</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>2</v>
@@ -2325,12 +2324,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="D3" s="0" t="n">
-        <v>2004</v>
+        <v>1997</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
@@ -2338,7 +2337,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>8</v>
@@ -2352,7 +2351,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -2369,7 +2368,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -2386,10 +2385,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -2403,15 +2402,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>104</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -2425,12 +2424,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
@@ -2447,7 +2446,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
@@ -2464,7 +2463,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -2481,10 +2480,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -2501,7 +2500,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -2518,7 +2517,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
@@ -2535,7 +2534,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="C17" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D37),ISNUMBER(D49)),SUM(D29,D37,D49),"")</f>
@@ -2552,7 +2551,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -2569,7 +2568,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -2586,7 +2585,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -2603,7 +2602,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -2620,15 +2619,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>118</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -2645,7 +2644,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -2662,7 +2661,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -2679,10 +2678,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>124</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -2696,25 +2695,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>129</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -2728,7 +2727,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -2745,7 +2744,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -2762,7 +2761,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -2779,7 +2778,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -2796,22 +2795,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -2828,22 +2827,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -2860,7 +2859,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -2877,7 +2876,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -2894,7 +2893,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -2907,7 +2906,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -2924,22 +2923,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -2956,22 +2955,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -2988,17 +2987,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -3015,17 +3014,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -3042,10 +3041,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C61" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>161</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -3059,17 +3058,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -3083,22 +3082,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -3115,17 +3114,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -3142,17 +3141,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -3166,12 +3165,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Fallback for formula errors during import
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="940" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="469" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables_W" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="179">
   <si>
     <t>Survey Category</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Code 2</t>
+  </si>
+  <si>
+    <t>&lt;= this cell has formula error (cyclic reference)</t>
+  </si>
+  <si>
+    <t>&lt;= this cell has formula error (wrong syntax)</t>
   </si>
   <si>
     <t>Survey name 1</t>
@@ -650,17 +656,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:W93"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D3" activeCellId="0" pane="topLeft" sqref="D3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="L1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="V2" activeCellId="0" pane="topLeft" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="15.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.6887755102041"/>
+    <col collapsed="false" hidden="false" max="18" min="2" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="11.6887755102041"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.9438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="11.6887755102041"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -683,13 +691,39 @@
         <f aca="false">$D$1</f>
         <v>Switzerland</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="0" t="str">
+        <f aca="false">$P$1</f>
+        <v/>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="0" t="e">
+        <f aca="false">2+</f>
+        <v>#N/A</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
@@ -702,39 +736,39 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="K4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -749,7 +783,7 @@
         <v>6.6</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>60</v>
@@ -763,7 +797,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -778,7 +812,7 @@
         <v>4.3</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J6" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J7),ISNUMBER(J8)),SUM(J7,J8),"")</f>
@@ -795,10 +829,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -810,26 +844,26 @@
         <v>4.3</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -841,23 +875,23 @@
         <v>2.3</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
@@ -872,7 +906,7 @@
         <v>82.6</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J11" s="0" t="n">
         <f aca="false">IF(SUMIF(G12:G53,"&gt;""",J12:J53)=0,"",SUMIF(G12:G53,"&gt;""",J12:J53))</f>
@@ -889,7 +923,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
@@ -904,7 +938,7 @@
         <v>74.6</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J12" s="0" t="n">
         <f aca="false">IF(SUMIF(G14:G17,"&gt;""",J14:J17)+SUMIF(G26:G29,"&gt;""",J26:J29)+SUMIF(G46:G49,"&gt;""",J46:J49)+SUMIF(G34:G37,"&gt;""",J34:J37)=0,"",SUMIF(G14:G17,"&gt;""",J14:J17)+SUMIF(G26:G29,"&gt;""",J26:J29)+SUMIF(G46:G49,"&gt;""",J46:J49)+SUMIF(G34:G37,"&gt;""",J34:J37))</f>
@@ -921,7 +955,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -936,7 +970,7 @@
         <v/>
       </c>
       <c r="I13" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J13" s="0" t="str">
         <f aca="false">IF(SUMIF(G18:G21,"&gt;""",J18:J21)+SUMIF(G38:G41,"&gt;""",J38:J41)+SUMIF(G50:G53,"&gt;""",J50:J53)=0,"",SUMIF(G18:G21,"&gt;""",J18:J21)+SUMIF(G38:G41,"&gt;""",J38:J41)+SUMIF(G50:G53,"&gt;""",J50:J53))</f>
@@ -953,7 +987,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="C14" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -968,7 +1002,7 @@
         <v>66.6</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(G26),ISTEXT(G34),ISTEXT(G46)),SUM(J26,J34,J46),IF(OR(ISNUMBER(J15),ISNUMBER(J16),ISNUMBER(J17)),SUM(J15,J16,J17),""))</f>
@@ -985,7 +1019,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -1000,7 +1034,7 @@
         <v/>
       </c>
       <c r="I15" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J27),ISNUMBER(J35),ISNUMBER(J47)),SUM(J27,J35,J47),"")</f>
@@ -1017,7 +1051,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
@@ -1032,7 +1066,7 @@
         <v/>
       </c>
       <c r="I16" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J28),ISNUMBER(J36),ISNUMBER(J48)),SUM(J28,J36,J48),"")</f>
@@ -1049,10 +1083,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">4*4</f>
@@ -1067,7 +1101,7 @@
         <v>8</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J29),ISNUMBER(J37),ISNUMBER(J49)),SUM(J29,J37,J49),"")</f>
@@ -1084,7 +1118,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -1099,7 +1133,7 @@
         <v/>
       </c>
       <c r="I18" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G38),ISTEXT(G50)),SUM(J38,J50),IF(OR(ISNUMBER(J19),ISNUMBER(J20),ISNUMBER(J21)),SUM(J19,J20,J21),""))</f>
@@ -1116,7 +1150,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -1131,7 +1165,7 @@
         <v/>
       </c>
       <c r="I19" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J39),ISNUMBER(J51)),SUM(J39,J51),"")</f>
@@ -1148,7 +1182,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -1163,7 +1197,7 @@
         <v/>
       </c>
       <c r="I20" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J40),ISNUMBER(J52)),SUM(J40,J52),"")</f>
@@ -1180,7 +1214,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -1195,7 +1229,7 @@
         <v/>
       </c>
       <c r="I21" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J41),ISNUMBER(J53)),SUM(J41,J53),"")</f>
@@ -1212,10 +1246,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="B22" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J22" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J23),ISNUMBER(J24),ISNUMBER(J25),ISNUMBER(J26),ISNUMBER(J27),ISNUMBER(J28),ISNUMBER(J29),ISNUMBER(J30),ISNUMBER(J31),ISNUMBER(J32),ISNUMBER(J33),ISNUMBER(J34),ISNUMBER(J35),ISNUMBER(J36),ISNUMBER(J37),ISNUMBER(J38),ISNUMBER(J39),ISNUMBER(J40),ISNUMBER(J41)),SUMIF(G23:G41,"&gt;""",J23:J41),"")</f>
@@ -1232,7 +1266,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -1247,7 +1281,7 @@
         <v/>
       </c>
       <c r="I23" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J27),ISNUMBER(J31)),SUM(J27,J31),"")</f>
@@ -1264,7 +1298,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -1279,7 +1313,7 @@
         <v/>
       </c>
       <c r="I24" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J28),ISNUMBER(J32)),SUM(J28,J32),"")</f>
@@ -1296,7 +1330,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -1311,7 +1345,7 @@
         <v/>
       </c>
       <c r="I25" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J29),ISNUMBER(J33)),SUM(J29,J33),"")</f>
@@ -1328,10 +1362,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -1343,10 +1377,10 @@
         <v>66.6</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>22</v>
@@ -1360,34 +1394,34 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -1399,10 +1433,10 @@
         <v>8</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>1</v>
@@ -1416,7 +1450,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -1431,7 +1465,7 @@
         <v/>
       </c>
       <c r="I31" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J35),ISNUMBER(J39)),SUM(J35,J39),"")</f>
@@ -1448,7 +1482,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -1463,7 +1497,7 @@
         <v/>
       </c>
       <c r="I32" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J36),ISNUMBER(J40)),SUM(J36,J40),"")</f>
@@ -1480,7 +1514,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -1495,7 +1529,7 @@
         <v/>
       </c>
       <c r="I33" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J37),ISNUMBER(J41)),SUM(J37,J41),"")</f>
@@ -1512,7 +1546,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -1527,7 +1561,7 @@
         <v/>
       </c>
       <c r="I34" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G35),ISTEXT(G36),ISTEXT(G37)),SUM(J35,J36,J37),"")</f>
@@ -1544,31 +1578,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -1583,7 +1617,7 @@
         <v/>
       </c>
       <c r="I38" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G39),ISTEXT(G40),ISTEXT(G41)),SUM(J39,J40,J41),"")</f>
@@ -1600,31 +1634,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -1639,7 +1673,7 @@
         <v/>
       </c>
       <c r="I42" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J43),ISNUMBER(J44),ISNUMBER(J45),ISNUMBER(J46),ISNUMBER(J47),ISNUMBER(J48),ISNUMBER(J49),ISNUMBER(J50),ISNUMBER(J51),ISNUMBER(J52),ISNUMBER(J53)),SUMIF(G43:G53,"&gt;""",J43:J53),"")</f>
@@ -1656,7 +1690,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -1671,7 +1705,7 @@
         <v/>
       </c>
       <c r="I43" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J47),ISNUMBER(J51)),SUM(J47,J51),"")</f>
@@ -1688,7 +1722,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -1703,7 +1737,7 @@
         <v/>
       </c>
       <c r="H44" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J48),ISNUMBER(J52)),SUM(J48,J52),"")</f>
@@ -1720,7 +1754,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -1731,7 +1765,7 @@
         <v/>
       </c>
       <c r="I45" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(K49),ISNUMBER(K53)),SUM(K49,K53),"")</f>
@@ -1744,7 +1778,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -1759,7 +1793,7 @@
         <v/>
       </c>
       <c r="I46" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G47),ISTEXT(G48),ISTEXT(G49)),SUM(J47,J48,J49),"")</f>
@@ -1776,31 +1810,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -1815,7 +1849,7 @@
         <v/>
       </c>
       <c r="I50" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G51),ISTEXT(G52),ISTEXT(G53)),SUM(J51,J52,J53),"")</f>
@@ -1832,31 +1866,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -1871,7 +1905,7 @@
         <v/>
       </c>
       <c r="I54" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J55),ISNUMBER(J56)),SUM(J55,J56),"")</f>
@@ -1888,23 +1922,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -1919,7 +1953,7 @@
         <v/>
       </c>
       <c r="I57" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J58),ISNUMBER(J59)),SUM(J58,J59),"")</f>
@@ -1936,23 +1970,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -1967,7 +2001,7 @@
         <v>9.8</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J60" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J61),ISNUMBER(J62),ISNUMBER(J63),ISNUMBER(J64),ISNUMBER(J65),ISNUMBER(J66),ISNUMBER(J67)),SUM(J61:J67),"")</f>
@@ -1984,10 +2018,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -1999,31 +2033,31 @@
         <v>7</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -2035,36 +2069,36 @@
         <v>2.8</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -2079,7 +2113,7 @@
         <v/>
       </c>
       <c r="I68" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J69),ISNUMBER(J70)),SUM(J69,J70),"")</f>
@@ -2096,23 +2130,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -2127,7 +2161,7 @@
         <v>0.1</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J72),ISNUMBER(J73),ISNUMBER(J74),ISNUMBER(J75)),SUM(J72:J75),"")</f>
@@ -2144,23 +2178,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -2172,7 +2206,7 @@
         <v>0.1</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J74" s="0" t="n">
         <v>5</v>
@@ -2186,15 +2220,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -2206,12 +2240,12 @@
         <v>0.1</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="77">
       <c r="B77" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D5),ISNUMBER(D11),ISNUMBER(D54),ISNUMBER(D57),ISNUMBER(D60),ISNUMBER(D71),ISNUMBER(D76)),SUM(D5,D11,D54,D57,D60,D68,D71,D76),"")</f>
@@ -2226,7 +2260,7 @@
         <v>99.2</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J5),ISNUMBER(J11),ISNUMBER(J54),ISNUMBER(J57),ISNUMBER(J60),ISNUMBER(J71),ISNUMBER(J76)),SUM(J5,J11,J54,J57,J60,J68,J71,J76),"")</f>
@@ -2243,21 +2277,21 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="91">
       <c r="D91" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="D92" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
@@ -2274,10 +2308,10 @@
         <v>No</v>
       </c>
       <c r="J93" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K93" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2298,8 +2332,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A67" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F100" activeCellId="0" pane="topLeft" sqref="F100"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2311,7 +2345,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
@@ -2322,7 +2356,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
@@ -2332,24 +2366,24 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -2366,7 +2400,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -2383,10 +2417,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -2400,15 +2434,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -2422,12 +2456,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
@@ -2444,7 +2478,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
@@ -2461,7 +2495,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -2478,10 +2512,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -2498,7 +2532,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -2515,7 +2549,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
@@ -2532,7 +2566,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="C17" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D37),ISNUMBER(D49)),SUM(D29,D37,D49),"")</f>
@@ -2549,7 +2583,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -2566,7 +2600,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -2583,7 +2617,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -2600,7 +2634,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -2617,15 +2651,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -2642,7 +2676,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -2659,7 +2693,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -2676,10 +2710,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -2693,25 +2727,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -2725,7 +2759,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -2742,7 +2776,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -2759,7 +2793,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -2776,7 +2810,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -2793,22 +2827,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -2825,22 +2859,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -2857,7 +2891,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -2874,7 +2908,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -2891,7 +2925,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -2904,7 +2938,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -2921,22 +2955,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -2953,22 +2987,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -2985,17 +3019,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -3012,17 +3046,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -3039,10 +3073,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -3056,17 +3090,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -3080,22 +3114,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -3112,17 +3146,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -3139,17 +3173,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -3163,12 +3197,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -3182,7 +3216,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="77">
       <c r="B77" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D5),ISNUMBER(D11),ISNUMBER(D54),ISNUMBER(D57),ISNUMBER(D60),ISNUMBER(D71),ISNUMBER(D76)),SUM(D5,D11,D54,D57,D60,D68,D71,D76),"")</f>
@@ -3199,33 +3233,33 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="96">
       <c r="D96" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="97">
       <c r="E97" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="98">
       <c r="F98" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="99">
       <c r="D99" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
       <c r="B100" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>0.1</v>

</xml_diff>

<commit_message>
Import estimates from Excel files
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="469" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="940" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables_W" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="182">
   <si>
     <t>Survey Category</t>
   </si>
@@ -296,6 +296,15 @@
   </si>
   <si>
     <t>Cat 4-32</t>
+  </si>
+  <si>
+    <t>estimate rule 1</t>
+  </si>
+  <si>
+    <t>not imported</t>
+  </si>
+  <si>
+    <t>estimate rule 2 for surface water</t>
   </si>
   <si>
     <t>No</t>
@@ -658,8 +667,8 @@
   </sheetPr>
   <dimension ref="A1:W93"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="L1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="V2" activeCellId="0" pane="topLeft" sqref="V2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A64" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B84" activeCellId="0" pane="topLeft" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2275,23 +2284,50 @@
         <v>70</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
+      <c r="B83" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <f aca="false">0.3+0.4</f>
+        <v>0.7</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <f aca="false">0.8+0.1</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
+      <c r="B84" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
+      <c r="B87" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <f aca="false">0.2+0.3</f>
+        <v>0.5</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="91">
       <c r="D91" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="D92" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E92" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
@@ -2308,10 +2344,10 @@
         <v>No</v>
       </c>
       <c r="J93" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="K93" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2333,7 +2369,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B84 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2345,7 +2381,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
@@ -2356,7 +2392,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
@@ -2369,7 +2405,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>10</v>
@@ -2383,7 +2419,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -2400,7 +2436,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -2417,10 +2453,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -2434,15 +2470,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -2456,12 +2492,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
@@ -2478,7 +2514,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
@@ -2495,7 +2531,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -2512,10 +2548,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -2532,7 +2568,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -2549,7 +2585,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
@@ -2566,7 +2602,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="C17" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D37),ISNUMBER(D49)),SUM(D29,D37,D49),"")</f>
@@ -2583,7 +2619,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -2600,7 +2636,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -2617,7 +2653,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -2634,7 +2670,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -2651,15 +2687,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -2676,7 +2712,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -2693,7 +2729,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -2710,10 +2746,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -2727,25 +2763,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -2759,7 +2795,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -2776,7 +2812,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -2793,7 +2829,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -2810,7 +2846,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -2827,22 +2863,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -2859,22 +2895,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -2891,7 +2927,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -2908,7 +2944,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -2925,7 +2961,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -2938,7 +2974,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -2955,22 +2991,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -2987,22 +3023,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -3019,17 +3055,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -3046,17 +3082,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -3073,10 +3109,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -3090,17 +3126,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -3114,22 +3150,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -3146,17 +3182,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -3173,17 +3209,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -3197,12 +3233,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -3233,33 +3269,33 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="96">
       <c r="D96" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="97">
       <c r="E97" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="98">
       <c r="F98" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="99">
       <c r="D99" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
       <c r="B100" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>0.1</v>

</xml_diff>

<commit_message>
Import Calculations, Estimates and Ratios as converted formulas
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="186">
   <si>
     <t>Survey Category</t>
   </si>
@@ -304,6 +304,12 @@
     <t>not imported</t>
   </si>
   <si>
+    <t>cross questionnaire formula</t>
+  </si>
+  <si>
+    <t>not duplicated</t>
+  </si>
+  <si>
     <t>estimate rule 2 for surface water</t>
   </si>
   <si>
@@ -320,6 +326,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>ratio (independent)</t>
+  </si>
+  <si>
+    <t>ratio referenced by estimate</t>
   </si>
   <si>
     <t>B Survey Category</t>
@@ -660,15 +672,1389 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="0" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3849840" y="11460240"/>
+          <a:ext cx="0" cy="2209320"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3849840" y="11460240"/>
+          <a:ext cx="6446520" cy="2209320"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3849840" y="13669560"/>
+          <a:ext cx="0" cy="1543680"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3849840" y="11460240"/>
+          <a:ext cx="0" cy="162720"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3849840" y="11460240"/>
+          <a:ext cx="0" cy="325080"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3849840" y="11460240"/>
+          <a:ext cx="0" cy="487800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3849840" y="11460240"/>
+          <a:ext cx="0" cy="650160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10296360" y="11460240"/>
+          <a:ext cx="0" cy="162720"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10296360" y="11460240"/>
+          <a:ext cx="0" cy="325080"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10296360" y="11460240"/>
+          <a:ext cx="0" cy="487800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10296360" y="11460240"/>
+          <a:ext cx="0" cy="650160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3849840" y="9834840"/>
+          <a:ext cx="0" cy="5378400"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3849840" y="9997200"/>
+          <a:ext cx="0" cy="5216040"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4924080" y="11460240"/>
+          <a:ext cx="0" cy="2209320"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4924080" y="11460240"/>
+          <a:ext cx="6446520" cy="2209320"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4924080" y="13669560"/>
+          <a:ext cx="0" cy="1543680"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5998680" y="11460240"/>
+          <a:ext cx="0" cy="2209320"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5998680" y="11460240"/>
+          <a:ext cx="6446520" cy="2209320"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5998680" y="13669560"/>
+          <a:ext cx="0" cy="1543680"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5998680" y="11460240"/>
+          <a:ext cx="0" cy="162720"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5998680" y="11460240"/>
+          <a:ext cx="0" cy="325080"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5998680" y="11460240"/>
+          <a:ext cx="0" cy="487800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5998680" y="11460240"/>
+          <a:ext cx="0" cy="650160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12445200" y="11460240"/>
+          <a:ext cx="0" cy="162720"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12445200" y="11460240"/>
+          <a:ext cx="0" cy="325080"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12445200" y="11460240"/>
+          <a:ext cx="0" cy="487800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12445200" y="11460240"/>
+          <a:ext cx="0" cy="650160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4924080" y="11460240"/>
+          <a:ext cx="0" cy="162720"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4924080" y="11460240"/>
+          <a:ext cx="0" cy="325080"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4924080" y="11460240"/>
+          <a:ext cx="0" cy="487800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4924080" y="11460240"/>
+          <a:ext cx="0" cy="650160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11370600" y="11460240"/>
+          <a:ext cx="0" cy="162720"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11370600" y="11460240"/>
+          <a:ext cx="0" cy="325080"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11370600" y="11460240"/>
+          <a:ext cx="0" cy="487800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11370600" y="11460240"/>
+          <a:ext cx="0" cy="650160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4924080" y="9834840"/>
+          <a:ext cx="0" cy="5378400"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4924080" y="9997200"/>
+          <a:ext cx="0" cy="5216040"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0000ff"/>
+          </a:solidFill>
+          <a:headEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W93"/>
+  <dimension ref="A1:W95"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A64" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B84" activeCellId="0" pane="topLeft" sqref="B84"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A61" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F95" activeCellId="0" pane="topLeft" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2302,9 +3688,43 @@
         <v>92</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
+      <c r="B85" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <f aca="false">D71+J71+D95</f>
+        <v>20.5</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <f aca="false">E71+K71+E95</f>
+        <v>7.1</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <f aca="false">F71+L71+F95</f>
+        <v>6.1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
+      <c r="B86" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <f aca="false">D74+D71</f>
+        <v>17</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <f aca="false">E74+E71</f>
+        <v>0.2</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <f aca="false">F74+F71</f>
+        <v>0.2</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
       <c r="B87" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E87" s="0" t="n">
         <f aca="false">0.2+0.3</f>
@@ -2313,21 +3733,21 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="91">
       <c r="D91" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="D92" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
@@ -2344,10 +3764,32 @@
         <v>No</v>
       </c>
       <c r="J93" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K93" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
+      <c r="B94" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <f aca="false">D60+D61</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
+      <c r="B95" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <f aca="false">D61+D62</f>
+        <v>7</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <f aca="false">E61+E62</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2358,6 +3800,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2369,7 +3812,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B84 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2381,7 +3824,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
@@ -2392,7 +3835,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
@@ -2405,7 +3848,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>10</v>
@@ -2419,7 +3862,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -2436,7 +3879,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -2453,10 +3896,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -2470,15 +3913,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -2492,12 +3935,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
@@ -2514,7 +3957,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
@@ -2531,7 +3974,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -2548,10 +3991,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -2568,7 +4011,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -2585,7 +4028,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
@@ -2602,7 +4045,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="C17" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D37),ISNUMBER(D49)),SUM(D29,D37,D49),"")</f>
@@ -2619,7 +4062,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -2636,7 +4079,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -2653,7 +4096,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -2670,7 +4113,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -2687,15 +4130,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -2712,7 +4155,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -2729,7 +4172,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -2746,10 +4189,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -2763,25 +4206,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -2795,7 +4238,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -2812,7 +4255,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -2829,7 +4272,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -2846,7 +4289,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -2863,22 +4306,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -2895,22 +4338,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -2927,7 +4370,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -2944,7 +4387,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -2961,7 +4404,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -2974,7 +4417,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -2991,22 +4434,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -3023,22 +4466,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -3055,17 +4498,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -3082,17 +4525,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -3109,10 +4552,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -3126,17 +4569,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -3150,22 +4593,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -3182,17 +4625,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -3209,17 +4652,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -3233,12 +4676,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -3269,33 +4712,33 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="96">
       <c r="D96" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="97">
       <c r="E97" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="98">
       <c r="F98" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="99">
       <c r="D99" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
       <c r="B100" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>0.1</v>

</xml_diff>

<commit_message>
Import high filters' formulas
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="188">
   <si>
     <t>Survey Category</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>estimate rule 2 for surface water</t>
+  </si>
+  <si>
+    <t>improved water</t>
+  </si>
+  <si>
+    <t>piped onto premises</t>
   </si>
   <si>
     <t>No</t>
@@ -2053,8 +2059,8 @@
   </sheetPr>
   <dimension ref="A1:W95"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A61" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F95" activeCellId="0" pane="topLeft" sqref="F95"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A65" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D89" activeCellId="0" pane="topLeft" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -3731,23 +3737,37 @@
         <v>0.5</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
+      <c r="A89" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <f aca="false">D86+D71</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
+      <c r="A90" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="91">
       <c r="D91" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="D92" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
@@ -3764,15 +3784,15 @@
         <v>No</v>
       </c>
       <c r="J93" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="K93" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
       <c r="B94" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D94" s="0" t="n">
         <f aca="false">D60+D61</f>
@@ -3781,7 +3801,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
       <c r="B95" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D95" s="0" t="n">
         <f aca="false">D61+D62</f>
@@ -3811,8 +3831,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A71" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C93" activeCellId="0" pane="topLeft" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3824,7 +3844,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
@@ -3835,7 +3855,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
@@ -3848,7 +3868,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>10</v>
@@ -3862,7 +3882,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -3879,7 +3899,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -3896,10 +3916,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -3913,15 +3933,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -3935,12 +3955,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
@@ -3957,7 +3977,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
@@ -3974,7 +3994,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -3991,10 +4011,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -4011,7 +4031,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -4028,7 +4048,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
@@ -4045,7 +4065,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="C17" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D37),ISNUMBER(D49)),SUM(D29,D37,D49),"")</f>
@@ -4062,7 +4082,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -4079,7 +4099,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -4096,7 +4116,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -4113,7 +4133,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -4130,15 +4150,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -4155,7 +4175,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -4172,7 +4192,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -4189,10 +4209,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -4206,25 +4226,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -4238,7 +4258,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -4255,7 +4275,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -4272,7 +4292,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -4289,7 +4309,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -4306,22 +4326,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -4338,22 +4358,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -4370,7 +4390,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -4387,7 +4407,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -4404,7 +4424,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -4417,7 +4437,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -4434,22 +4454,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -4466,22 +4486,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -4498,17 +4518,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -4525,17 +4545,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -4552,10 +4572,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -4569,17 +4589,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -4593,22 +4613,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -4625,17 +4645,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -4652,17 +4672,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -4676,12 +4696,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -4712,33 +4732,33 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="96">
       <c r="D96" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="97">
       <c r="E97" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="98">
       <c r="F98" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="99">
       <c r="D99" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
       <c r="B100" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>0.1</v>

</xml_diff>

<commit_message>
Support formula range syntax and unofficial filters references
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -683,15 +683,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -700,7 +700,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3849840" y="11460240"/>
+          <a:off x="3876840" y="11451240"/>
           <a:ext cx="0" cy="2209320"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -720,15 +720,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -737,7 +737,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3849840" y="11460240"/>
+          <a:off x="3876840" y="11451240"/>
           <a:ext cx="6446520" cy="2209320"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -757,15 +757,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -774,7 +774,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3849840" y="13669560"/>
+          <a:off x="3876840" y="13660560"/>
           <a:ext cx="0" cy="1543680"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -794,15 +794,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -811,7 +811,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3849840" y="11460240"/>
+          <a:off x="3876840" y="11451240"/>
           <a:ext cx="0" cy="162720"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -831,15 +831,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -848,7 +848,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3849840" y="11460240"/>
+          <a:off x="3876840" y="11451240"/>
           <a:ext cx="0" cy="325080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -868,15 +868,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -885,7 +885,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3849840" y="11460240"/>
+          <a:off x="3876840" y="11451240"/>
           <a:ext cx="0" cy="487800"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -905,15 +905,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -922,7 +922,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3849840" y="11460240"/>
+          <a:off x="3876840" y="11451240"/>
           <a:ext cx="0" cy="650160"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -942,15 +942,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -959,7 +959,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10296360" y="11460240"/>
+          <a:off x="10323360" y="11451240"/>
           <a:ext cx="0" cy="162720"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -979,15 +979,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -996,7 +996,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10296360" y="11460240"/>
+          <a:off x="10323360" y="11451240"/>
           <a:ext cx="0" cy="325080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1016,15 +1016,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1033,7 +1033,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10296360" y="11460240"/>
+          <a:off x="10323360" y="11451240"/>
           <a:ext cx="0" cy="487800"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1053,15 +1053,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1070,7 +1070,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10296360" y="11460240"/>
+          <a:off x="10323360" y="11451240"/>
           <a:ext cx="0" cy="650160"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1090,15 +1090,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1107,7 +1107,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3849840" y="9834840"/>
+          <a:off x="3876840" y="9825840"/>
           <a:ext cx="0" cy="5378400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1127,15 +1127,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1144,7 +1144,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3849840" y="9997200"/>
+          <a:off x="3876840" y="9988200"/>
           <a:ext cx="0" cy="5216040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1164,15 +1164,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1181,7 +1181,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4924080" y="11460240"/>
+          <a:off x="4951080" y="11451240"/>
           <a:ext cx="0" cy="2209320"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1201,15 +1201,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1218,7 +1218,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4924080" y="11460240"/>
+          <a:off x="4951080" y="11451240"/>
           <a:ext cx="6446520" cy="2209320"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1238,15 +1238,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1255,7 +1255,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4924080" y="13669560"/>
+          <a:off x="4951080" y="13660560"/>
           <a:ext cx="0" cy="1543680"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1275,15 +1275,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1292,7 +1292,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5998680" y="11460240"/>
+          <a:off x="6025680" y="11451240"/>
           <a:ext cx="0" cy="2209320"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1312,15 +1312,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1329,7 +1329,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5998680" y="11460240"/>
+          <a:off x="6025680" y="11451240"/>
           <a:ext cx="6446520" cy="2209320"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1349,15 +1349,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1366,7 +1366,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5998680" y="13669560"/>
+          <a:off x="6025680" y="13660560"/>
           <a:ext cx="0" cy="1543680"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1386,15 +1386,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1403,7 +1403,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5998680" y="11460240"/>
+          <a:off x="6025680" y="11451240"/>
           <a:ext cx="0" cy="162720"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1423,15 +1423,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1440,7 +1440,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5998680" y="11460240"/>
+          <a:off x="6025680" y="11451240"/>
           <a:ext cx="0" cy="325080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1460,15 +1460,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1477,7 +1477,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5998680" y="11460240"/>
+          <a:off x="6025680" y="11451240"/>
           <a:ext cx="0" cy="487800"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1497,15 +1497,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1514,7 +1514,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5998680" y="11460240"/>
+          <a:off x="6025680" y="11451240"/>
           <a:ext cx="0" cy="650160"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1534,15 +1534,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1551,7 +1551,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="12445200" y="11460240"/>
+          <a:off x="12472200" y="11451240"/>
           <a:ext cx="0" cy="162720"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1571,15 +1571,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1588,7 +1588,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="12445200" y="11460240"/>
+          <a:off x="12472200" y="11451240"/>
           <a:ext cx="0" cy="325080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1608,15 +1608,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1625,7 +1625,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="12445200" y="11460240"/>
+          <a:off x="12472200" y="11451240"/>
           <a:ext cx="0" cy="487800"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1645,15 +1645,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1662,7 +1662,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="12445200" y="11460240"/>
+          <a:off x="12472200" y="11451240"/>
           <a:ext cx="0" cy="650160"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1682,15 +1682,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1699,7 +1699,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4924080" y="11460240"/>
+          <a:off x="4951080" y="11451240"/>
           <a:ext cx="0" cy="162720"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1719,15 +1719,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1736,7 +1736,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4924080" y="11460240"/>
+          <a:off x="4951080" y="11451240"/>
           <a:ext cx="0" cy="325080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1756,15 +1756,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1773,7 +1773,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4924080" y="11460240"/>
+          <a:off x="4951080" y="11451240"/>
           <a:ext cx="0" cy="487800"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1793,15 +1793,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1810,7 +1810,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4924080" y="11460240"/>
+          <a:off x="4951080" y="11451240"/>
           <a:ext cx="0" cy="650160"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1830,15 +1830,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1847,7 +1847,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="11370600" y="11460240"/>
+          <a:off x="11397600" y="11451240"/>
           <a:ext cx="0" cy="162720"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1867,15 +1867,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1884,7 +1884,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="11370600" y="11460240"/>
+          <a:off x="11397600" y="11451240"/>
           <a:ext cx="0" cy="325080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1904,15 +1904,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1921,7 +1921,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="11370600" y="11460240"/>
+          <a:off x="11397600" y="11451240"/>
           <a:ext cx="0" cy="487800"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1941,15 +1941,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1958,7 +1958,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="11370600" y="11460240"/>
+          <a:off x="11397600" y="11451240"/>
           <a:ext cx="0" cy="650160"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1978,15 +1978,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1995,7 +1995,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4924080" y="9834840"/>
+          <a:off x="4951080" y="9825840"/>
           <a:ext cx="0" cy="5378400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2015,15 +2015,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2032,7 +2032,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4924080" y="9997200"/>
+          <a:off x="4951080" y="9988200"/>
           <a:ext cx="0" cy="5216040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2059,8 +2059,8 @@
   </sheetPr>
   <dimension ref="A1:W95"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A65" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D89" activeCellId="0" pane="topLeft" sqref="D89"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A57" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D87" activeCellId="0" pane="topLeft" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -3731,6 +3731,10 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
       <c r="B87" s="0" t="s">
         <v>95</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <f aca="false">IF(ISTEXT(A61), SUM(D71:D74),12345)</f>
+        <v>17</v>
       </c>
       <c r="E87" s="0" t="n">
         <f aca="false">0.2+0.3</f>

</xml_diff>

<commit_message>
Use array notation in formula when expanding range
This is necessary for instance for SUMIF(). SUM() can have as many arguments
as necessary, but SUMIF() can only have exactly 2 or 3 arguments. The workaround
to expend range and still use SUMIF() is to use array notation.

Also see http://office.microsoft.com/en-us/excel-help/more-arrays-introducing-array-constants-in-excel-HA001087291.aspx
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="940" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="469" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables_W" sheetId="1" state="visible" r:id="rId2"/>
@@ -636,6 +636,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="8"/>
     </font>
@@ -712,15 +713,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -729,7 +730,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3849840" y="7721280"/>
+          <a:off x="3876840" y="7712280"/>
           <a:ext cx="0" cy="6409080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -749,15 +750,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>102</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -766,7 +767,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="3849840" y="14130360"/>
+          <a:off x="3876840" y="14121360"/>
           <a:ext cx="6804720" cy="2305080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -793,8 +794,8 @@
   </sheetPr>
   <dimension ref="A1:W95"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A61" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G84" activeCellId="0" pane="topLeft" sqref="G84"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A64" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D87" activeCellId="0" pane="topLeft" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2571,8 +2572,8 @@
   </sheetPr>
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A68" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E48" activeCellId="0" pane="topLeft" sqref="E48"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A82" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E10" activeCellId="0" pane="topLeft" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>

</xml_diff>

<commit_message>
Add non-regression tests for computation on real data
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="469" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="234" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables_W" sheetId="1" state="visible" r:id="rId2"/>
@@ -708,85 +708,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>295560</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>295560</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>67680</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="Line 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3876840" y="7712280"/>
-          <a:ext cx="0" cy="6409080"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="0000ff"/>
-          </a:solidFill>
-          <a:headEnd len="med" type="triangle" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>295560</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>67680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>295560</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>67680</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="Line 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="3876840" y="14121360"/>
-          <a:ext cx="6804720" cy="2305080"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="0000ff"/>
-          </a:solidFill>
-          <a:headEnd len="med" type="triangle" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -794,8 +715,8 @@
   </sheetPr>
   <dimension ref="A1:W95"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A64" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D87" activeCellId="0" pane="topLeft" sqref="D87"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A64" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D95" activeCellId="0" pane="topLeft" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2572,8 +2493,8 @@
   </sheetPr>
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A82" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E10" activeCellId="0" pane="topLeft" sqref="E10"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A76" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="J103" activeCellId="0" pane="topLeft" sqref="J103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -3740,7 +3661,7 @@
       </c>
       <c r="D88" s="2" t="n">
         <f aca="false">D48*$J103</f>
-        <v>10</v>
+        <v>10.2</v>
       </c>
       <c r="H88" s="0" t="s">
         <v>188</v>
@@ -3819,8 +3740,8 @@
         <v>190</v>
       </c>
       <c r="J103" s="2" t="n">
-        <f aca="false">(J51+J53)/J48</f>
-        <v>5</v>
+        <f aca="false">(J51+J53)/J48+0.1</f>
+        <v>5.1</v>
       </c>
     </row>
   </sheetData>
@@ -3831,6 +3752,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Can import several questionnaires for a single survey #2126
We used to assume that imported surveys had only one questionnaire. This
is wrong for Russia (RLMS96). This commit allow to import several questionnaires
for a same survey that appears several time in Excel files.

It also means that from now on, we cannot re-import data to overwrite them,
because it will always create new questionnaires.
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="234" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="469" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables_W" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="191">
   <si>
     <t>Survey Category</t>
   </si>
@@ -46,7 +46,10 @@
     <t>Survey name 1</t>
   </si>
   <si>
-    <t>Survey name 2</t>
+    <t>Comments on questionnaire 1</t>
+  </si>
+  <si>
+    <t>Comments on questionnaire 2</t>
   </si>
   <si>
     <t>Original denomination</t>
@@ -341,9 +344,6 @@
   </si>
   <si>
     <t>B Survey Category</t>
-  </si>
-  <si>
-    <t>Survey name 3 B</t>
   </si>
   <si>
     <t>ClassifiB Cation</t>
@@ -715,8 +715,8 @@
   </sheetPr>
   <dimension ref="A1:W95"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A64" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D95" activeCellId="0" pane="topLeft" sqref="D95"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G4" activeCellId="0" pane="topLeft" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -742,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J1" s="0" t="str">
         <f aca="false">$D$1</f>
@@ -780,52 +780,58 @@
         <v>6</v>
       </c>
       <c r="G2" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="D3" s="0" t="n">
         <v>1997</v>
       </c>
+      <c r="G3" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="J3" s="0" t="n">
         <v>2003</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="L4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -840,7 +846,7 @@
         <v>6.6</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>60</v>
@@ -854,7 +860,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -869,7 +875,7 @@
         <v>4.3</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J6" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J7),ISNUMBER(J8)),SUM(J7,J8),"")</f>
@@ -886,10 +892,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -901,26 +907,26 @@
         <v>4.3</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -932,23 +938,23 @@
         <v>2.3</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
@@ -963,7 +969,7 @@
         <v>82.6</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J11" s="0" t="n">
         <f aca="false">IF(SUMIF(G12:G53,"&gt;""",J12:J53)=0,"",SUMIF(G12:G53,"&gt;""",J12:J53))</f>
@@ -980,7 +986,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
@@ -995,7 +1001,7 @@
         <v>74.6</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J12" s="0" t="n">
         <f aca="false">IF(SUMIF(G14:G17,"&gt;""",J14:J17)+SUMIF(G26:G29,"&gt;""",J26:J29)+SUMIF(G46:G49,"&gt;""",J46:J49)+SUMIF(G34:G37,"&gt;""",J34:J37)=0,"",SUMIF(G14:G17,"&gt;""",J14:J17)+SUMIF(G26:G29,"&gt;""",J26:J29)+SUMIF(G46:G49,"&gt;""",J46:J49)+SUMIF(G34:G37,"&gt;""",J34:J37))</f>
@@ -1012,7 +1018,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -1027,7 +1033,7 @@
         <v/>
       </c>
       <c r="I13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J13" s="0" t="str">
         <f aca="false">IF(SUMIF(G18:G21,"&gt;""",J18:J21)+SUMIF(G38:G41,"&gt;""",J38:J41)+SUMIF(G50:G53,"&gt;""",J50:J53)=0,"",SUMIF(G18:G21,"&gt;""",J18:J21)+SUMIF(G38:G41,"&gt;""",J38:J41)+SUMIF(G50:G53,"&gt;""",J50:J53))</f>
@@ -1044,7 +1050,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="C14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -1059,7 +1065,7 @@
         <v>66.6</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(G26),ISTEXT(G34),ISTEXT(G46)),SUM(J26,J34,J46),IF(OR(ISNUMBER(J15),ISNUMBER(J16),ISNUMBER(J17)),SUM(J15,J16,J17),""))</f>
@@ -1076,7 +1082,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -1091,7 +1097,7 @@
         <v/>
       </c>
       <c r="I15" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J27),ISNUMBER(J35),ISNUMBER(J47)),SUM(J27,J35,J47),"")</f>
@@ -1108,7 +1114,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
@@ -1123,7 +1129,7 @@
         <v/>
       </c>
       <c r="I16" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J28),ISNUMBER(J36),ISNUMBER(J48)),SUM(J28,J36,J48),"")</f>
@@ -1140,10 +1146,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">4*4</f>
@@ -1158,7 +1164,7 @@
         <v>8</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J29),ISNUMBER(J37),ISNUMBER(J49)),SUM(J29,J37,J49),"")</f>
@@ -1175,7 +1181,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -1190,7 +1196,7 @@
         <v/>
       </c>
       <c r="I18" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G38),ISTEXT(G50)),SUM(J38,J50),IF(OR(ISNUMBER(J19),ISNUMBER(J20),ISNUMBER(J21)),SUM(J19,J20,J21),""))</f>
@@ -1207,7 +1213,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -1222,7 +1228,7 @@
         <v/>
       </c>
       <c r="I19" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J39),ISNUMBER(J51)),SUM(J39,J51),"")</f>
@@ -1239,7 +1245,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -1254,7 +1260,7 @@
         <v/>
       </c>
       <c r="I20" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J40),ISNUMBER(J52)),SUM(J40,J52),"")</f>
@@ -1271,7 +1277,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -1286,7 +1292,7 @@
         <v/>
       </c>
       <c r="I21" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J41),ISNUMBER(J53)),SUM(J41,J53),"")</f>
@@ -1303,10 +1309,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="B22" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J22" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J23),ISNUMBER(J24),ISNUMBER(J25),ISNUMBER(J26),ISNUMBER(J27),ISNUMBER(J28),ISNUMBER(J29),ISNUMBER(J30),ISNUMBER(J31),ISNUMBER(J32),ISNUMBER(J33),ISNUMBER(J34),ISNUMBER(J35),ISNUMBER(J36),ISNUMBER(J37),ISNUMBER(J38),ISNUMBER(J39),ISNUMBER(J40),ISNUMBER(J41)),SUMIF(G23:G41,"&gt;""",J23:J41),"")</f>
@@ -1323,7 +1329,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -1338,7 +1344,7 @@
         <v/>
       </c>
       <c r="I23" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J27),ISNUMBER(J31)),SUM(J27,J31),"")</f>
@@ -1355,7 +1361,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -1370,7 +1376,7 @@
         <v/>
       </c>
       <c r="I24" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J28),ISNUMBER(J32)),SUM(J28,J32),"")</f>
@@ -1387,7 +1393,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -1402,7 +1408,7 @@
         <v/>
       </c>
       <c r="I25" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J29),ISNUMBER(J33)),SUM(J29,J33),"")</f>
@@ -1419,10 +1425,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -1434,10 +1440,10 @@
         <v>66.6</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>22</v>
@@ -1451,34 +1457,34 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -1490,10 +1496,10 @@
         <v>8</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>1</v>
@@ -1507,7 +1513,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -1522,7 +1528,7 @@
         <v/>
       </c>
       <c r="I31" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J35),ISNUMBER(J39)),SUM(J35,J39),"")</f>
@@ -1539,7 +1545,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -1554,7 +1560,7 @@
         <v/>
       </c>
       <c r="I32" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J36),ISNUMBER(J40)),SUM(J36,J40),"")</f>
@@ -1571,7 +1577,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -1586,7 +1592,7 @@
         <v/>
       </c>
       <c r="I33" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J37),ISNUMBER(J41)),SUM(J37,J41),"")</f>
@@ -1603,7 +1609,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -1618,7 +1624,7 @@
         <v/>
       </c>
       <c r="I34" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G35),ISTEXT(G36),ISTEXT(G37)),SUM(J35,J36,J37),"")</f>
@@ -1635,31 +1641,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -1674,7 +1680,7 @@
         <v/>
       </c>
       <c r="I38" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G39),ISTEXT(G40),ISTEXT(G41)),SUM(J39,J40,J41),"")</f>
@@ -1691,31 +1697,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -1730,7 +1736,7 @@
         <v/>
       </c>
       <c r="I42" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J43),ISNUMBER(J44),ISNUMBER(J45),ISNUMBER(J46),ISNUMBER(J47),ISNUMBER(J48),ISNUMBER(J49),ISNUMBER(J50),ISNUMBER(J51),ISNUMBER(J52),ISNUMBER(J53)),SUMIF(G43:G53,"&gt;""",J43:J53),"")</f>
@@ -1747,7 +1753,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -1762,7 +1768,7 @@
         <v/>
       </c>
       <c r="I43" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J47),ISNUMBER(J51)),SUM(J47,J51),"")</f>
@@ -1779,7 +1785,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -1794,7 +1800,7 @@
         <v/>
       </c>
       <c r="H44" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J48),ISNUMBER(J52)),SUM(J48,J52),"")</f>
@@ -1811,7 +1817,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -1822,7 +1828,7 @@
         <v/>
       </c>
       <c r="I45" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(K49),ISNUMBER(K53)),SUM(K49,K53),"")</f>
@@ -1835,7 +1841,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -1850,7 +1856,7 @@
         <v/>
       </c>
       <c r="I46" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G47),ISTEXT(G48),ISTEXT(G49)),SUM(J47,J48,J49),"")</f>
@@ -1867,31 +1873,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -1906,7 +1912,7 @@
         <v/>
       </c>
       <c r="I50" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G51),ISTEXT(G52),ISTEXT(G53)),SUM(J51,J52,J53),"")</f>
@@ -1923,31 +1929,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -1962,7 +1968,7 @@
         <v/>
       </c>
       <c r="I54" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J55),ISNUMBER(J56)),SUM(J55,J56),"")</f>
@@ -1979,23 +1985,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -2010,7 +2016,7 @@
         <v/>
       </c>
       <c r="I57" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J58),ISNUMBER(J59)),SUM(J58,J59),"")</f>
@@ -2027,23 +2033,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -2058,7 +2064,7 @@
         <v>9.8</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J60" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J61),ISNUMBER(J62),ISNUMBER(J63),ISNUMBER(J64),ISNUMBER(J65),ISNUMBER(J66),ISNUMBER(J67)),SUM(J61:J67),"")</f>
@@ -2075,10 +2081,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -2090,31 +2096,31 @@
         <v>7</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -2126,36 +2132,36 @@
         <v>2.8</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -2170,7 +2176,7 @@
         <v/>
       </c>
       <c r="I68" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J69),ISNUMBER(J70)),SUM(J69,J70),"")</f>
@@ -2187,23 +2193,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -2218,7 +2224,7 @@
         <v>0.1</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J72),ISNUMBER(J73),ISNUMBER(J74),ISNUMBER(J75)),SUM(J72:J75),"")</f>
@@ -2235,23 +2241,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -2263,7 +2269,7 @@
         <v>0.1</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J74" s="0" t="n">
         <v>5</v>
@@ -2277,15 +2283,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -2297,12 +2303,12 @@
         <v>0.1</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="77">
       <c r="B77" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D5),ISNUMBER(D11),ISNUMBER(D54),ISNUMBER(D57),ISNUMBER(D60),ISNUMBER(D71),ISNUMBER(D76)),SUM(D5,D11,D54,D57,D60,D68,D71,D76),"")</f>
@@ -2317,7 +2323,7 @@
         <v>99.2</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J5),ISNUMBER(J11),ISNUMBER(J54),ISNUMBER(J57),ISNUMBER(J60),ISNUMBER(J71),ISNUMBER(J76)),SUM(J5,J11,J54,J57,J60,J68,J71,J76),"")</f>
@@ -2337,7 +2343,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
       <c r="B83" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D83" s="0" t="n">
         <f aca="false">0.3+0.4</f>
@@ -2350,12 +2356,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
       <c r="B84" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
       <c r="B85" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D85" s="0" t="n">
         <f aca="false">D71+J71+D95</f>
@@ -2372,7 +2378,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
       <c r="B86" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D86" s="0" t="n">
         <f aca="false">D74+D71</f>
@@ -2389,7 +2395,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
       <c r="B87" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D87" s="0" t="n">
         <f aca="false">IF(ISTEXT(A61), SUM(D71:D74),12345)</f>
@@ -2402,7 +2408,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D89" s="0" t="n">
         <f aca="false">D86+D71</f>
@@ -2411,26 +2417,26 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
       <c r="A90" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="91">
       <c r="D91" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="D92" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
@@ -2447,15 +2453,15 @@
         <v>No</v>
       </c>
       <c r="J93" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K93" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
       <c r="B94" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D94" s="0" t="n">
         <f aca="false">D60+D61</f>
@@ -2464,7 +2470,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
       <c r="B95" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D95" s="0" t="n">
         <f aca="false">D61+D62</f>
@@ -2493,8 +2499,8 @@
   </sheetPr>
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A76" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="J103" activeCellId="0" pane="topLeft" sqref="J103"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2508,7 +2514,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
@@ -2517,10 +2523,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>2</v>
@@ -2528,10 +2534,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>106</v>
+        <v>6</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>106</v>
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
@@ -2544,34 +2550,34 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>107</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>107</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
@@ -3625,7 +3631,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="77">
       <c r="B77" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D5),ISNUMBER(D11),ISNUMBER(D54),ISNUMBER(D57),ISNUMBER(D60),ISNUMBER(D71),ISNUMBER(D76)),SUM(D5,D11,D54,D57,D60,D68,D71,D76),"")</f>
@@ -3640,7 +3646,7 @@
         <v>157.8</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J77" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J5),ISNUMBER(J11),ISNUMBER(J54),ISNUMBER(J57),ISNUMBER(J60),ISNUMBER(J71),ISNUMBER(J76)),SUM(J5,J11,J54,J57,J60,J68,J71,J76),"")</f>
@@ -3673,46 +3679,46 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
       <c r="D96" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J96" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="97">
       <c r="E97" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K97" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98">
       <c r="F98" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L98" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99">
       <c r="D99" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K99" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L99" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">

</xml_diff>

<commit_message>
Don't assume symmetric questionnaires #2354
We used to assume that questionnaire on Tables_W and Tables_S was
always same questionnaire. But this is not the case at least for
Austria. We know double-check if the survey is also the same, thus
allowing to create new questionnaires even on Tables_S
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="469" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="234" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables_W" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="192">
   <si>
     <t>Survey Category</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>B Survey Category</t>
+  </si>
+  <si>
+    <t>Code 3</t>
   </si>
   <si>
     <t>ClassifiB Cation</t>
@@ -715,14 +718,18 @@
   </sheetPr>
   <dimension ref="A1:W95"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G4" activeCellId="0" pane="topLeft" sqref="G4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="P3" activeCellId="0" pane="topLeft" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3010204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="2" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="7.49489795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="7.49489795918367"/>
+    <col collapsed="false" hidden="false" max="18" min="13" style="0" width="15.2295918367347"/>
     <col collapsed="false" hidden="false" max="21" min="19" style="0" width="11.6887755102041"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.9438775510204"/>
     <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="11.6887755102041"/>
@@ -2499,16 +2506,18 @@
   </sheetPr>
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="I3" activeCellId="0" pane="topLeft" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="7.21938775510204"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.3010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="7.21938775510204"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.6887755102041"/>
   </cols>
   <sheetData>
@@ -2526,7 +2535,7 @@
         <v>106</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>2</v>
@@ -2553,7 +2562,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>11</v>
@@ -2568,7 +2577,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>11</v>
@@ -2582,7 +2591,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -2599,7 +2608,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -2614,15 +2623,15 @@
         <v>4.3</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -2634,23 +2643,23 @@
         <v>4.3</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -2662,20 +2671,20 @@
         <v>2.3</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
@@ -2692,7 +2701,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
@@ -2707,12 +2716,12 @@
         <v>133.2</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -2727,15 +2736,15 @@
         <v/>
       </c>
       <c r="I13" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -2750,12 +2759,12 @@
         <v>66.6</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -2770,12 +2779,12 @@
         <v/>
       </c>
       <c r="I15" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
@@ -2790,12 +2799,12 @@
         <v/>
       </c>
       <c r="I16" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="C17" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D37),ISNUMBER(D49)),SUM(D29,D37,D49),"")</f>
@@ -2810,12 +2819,12 @@
         <v/>
       </c>
       <c r="I17" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -2830,12 +2839,12 @@
         <v/>
       </c>
       <c r="I18" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -2850,12 +2859,12 @@
         <v/>
       </c>
       <c r="I19" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -2870,12 +2879,12 @@
         <v/>
       </c>
       <c r="I20" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -2890,20 +2899,20 @@
         <v/>
       </c>
       <c r="I21" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -2918,12 +2927,12 @@
         <v/>
       </c>
       <c r="I23" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -2938,12 +2947,12 @@
         <v/>
       </c>
       <c r="I24" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -2958,15 +2967,15 @@
         <v/>
       </c>
       <c r="I25" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -2978,39 +2987,39 @@
         <v>66.6</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -3022,12 +3031,12 @@
         <v>8</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -3042,12 +3051,12 @@
         <v/>
       </c>
       <c r="I31" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -3062,12 +3071,12 @@
         <v/>
       </c>
       <c r="I32" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -3082,12 +3091,12 @@
         <v/>
       </c>
       <c r="I33" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -3102,36 +3111,36 @@
         <v/>
       </c>
       <c r="I34" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -3146,36 +3155,36 @@
         <v/>
       </c>
       <c r="I38" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D42" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -3190,12 +3199,12 @@
         <v/>
       </c>
       <c r="I42" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -3210,12 +3219,12 @@
         <v/>
       </c>
       <c r="I43" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D44" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -3232,7 +3241,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -3243,12 +3252,12 @@
         <v/>
       </c>
       <c r="I45" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -3263,26 +3272,26 @@
         <v/>
       </c>
       <c r="I46" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J48" s="0" t="n">
         <v>0.1</v>
@@ -3290,15 +3299,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -3313,15 +3322,15 @@
         <v/>
       </c>
       <c r="I50" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J51" s="0" t="n">
         <v>0.3</v>
@@ -3329,18 +3338,18 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J53" s="0" t="n">
         <v>0.2</v>
@@ -3348,7 +3357,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -3363,28 +3372,28 @@
         <v/>
       </c>
       <c r="I54" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -3399,28 +3408,28 @@
         <v/>
       </c>
       <c r="I57" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -3435,15 +3444,15 @@
         <v>9.8</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -3455,28 +3464,28 @@
         <v>7</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -3488,36 +3497,36 @@
         <v>2.8</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -3532,28 +3541,28 @@
         <v/>
       </c>
       <c r="I68" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -3568,28 +3577,28 @@
         <v>0.1</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -3601,20 +3610,20 @@
         <v>0.1</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -3626,7 +3635,7 @@
         <v>0.1</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="77">
@@ -3663,14 +3672,14 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
       <c r="B88" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D88" s="2" t="n">
         <f aca="false">D48*$J103</f>
         <v>10.2</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J88" s="2" t="n">
         <f aca="false">J48*$CJ103</f>
@@ -3723,7 +3732,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
       <c r="B100" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>0.1</v>
@@ -3732,7 +3741,7 @@
         <v>0.25</v>
       </c>
       <c r="H100" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J100" s="0" t="n">
         <v>0.1</v>
@@ -3743,7 +3752,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
       <c r="H103" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J103" s="2" t="n">
         <f aca="false">(J51+J53)/J48+0.1</f>

</xml_diff>

<commit_message>
Prevent a Filter to be used more than once within same Survey #2689
Instead of duplicated use of Filter within a same Survey, we now should
use alternateNames of Questions
</commit_message>
<xml_diff>
--- a/tests/data/import_jmp.xlsx
+++ b/tests/data/import_jmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="234" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="234" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables_W" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="193">
   <si>
     <t>Survey Category</t>
   </si>
@@ -154,10 +154,13 @@
     <t>Cat 3-7</t>
   </si>
   <si>
-    <t>Alternate Cat 3-8</t>
+    <t>Alternate Cat 3-8 first</t>
   </si>
   <si>
     <t>Cat 3-8</t>
+  </si>
+  <si>
+    <t>Alternate Cat 3-8 second</t>
   </si>
   <si>
     <t>Cat 3-9</t>
@@ -606,42 +609,42 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="6">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF800000"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="8"/>
     </font>
   </fonts>
   <fills count="2">
@@ -653,7 +656,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -662,51 +665,51 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -718,8 +721,8 @@
   </sheetPr>
   <dimension ref="A1:W95"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="P3" activeCellId="0" pane="topLeft" sqref="P3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -735,7 +738,7 @@
     <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="11.6887755102041"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -782,7 +785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
@@ -790,7 +793,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -804,7 +807,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
@@ -836,7 +839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>14</v>
       </c>
@@ -865,7 +868,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
         <v>15</v>
       </c>
@@ -897,7 +900,7 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>16</v>
       </c>
@@ -920,7 +923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
         <v>18</v>
       </c>
@@ -928,7 +931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>19</v>
       </c>
@@ -951,7 +954,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
         <v>21</v>
       </c>
@@ -959,7 +962,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>22</v>
       </c>
@@ -991,7 +994,7 @@
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
         <v>23</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>55</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
         <v>24</v>
       </c>
@@ -1055,7 +1058,7 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
         <v>25</v>
       </c>
@@ -1087,7 +1090,7 @@
         <v>55</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
         <v>26</v>
       </c>
@@ -1119,39 +1122,51 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="0" t="str">
+      <c r="D16" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
-        <v/>
-      </c>
-      <c r="E16" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E28),ISNUMBER(E36),ISNUMBER(E48)),SUM(E28,E36,E48),"")</f>
-        <v/>
-      </c>
-      <c r="F16" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F28),ISNUMBER(F36),ISNUMBER(F48)),SUM(F28,F36,F48),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I16" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="0" t="str">
+      <c r="J16" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(J28),ISNUMBER(J36),ISNUMBER(J48)),SUM(J28,J36,J48),"")</f>
-        <v/>
-      </c>
-      <c r="K16" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K16" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(K28),ISNUMBER(K36),ISNUMBER(K48)),SUM(K28,K36,K48),"")</f>
-        <v/>
-      </c>
-      <c r="L16" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L16" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(L28),ISNUMBER(L36),ISNUMBER(L48)),SUM(L28,L36,L48),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>28</v>
       </c>
@@ -1173,20 +1188,26 @@
       <c r="I17" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="0" t="str">
+      <c r="J17" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(J29),ISNUMBER(J37),ISNUMBER(J49)),SUM(J29,J37,J49),"")</f>
-        <v/>
-      </c>
-      <c r="K17" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K17" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(K29),ISNUMBER(K37),ISNUMBER(K49)),SUM(K29,K37,K49),"")</f>
-        <v/>
-      </c>
-      <c r="L17" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L17" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(L29),ISNUMBER(L37),ISNUMBER(L49)),SUM(L29,L37,L49),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
         <v>30</v>
       </c>
@@ -1198,9 +1219,9 @@
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(E38,E50),IF(OR(ISNUMBER(E19),ISNUMBER(E20),ISNUMBER(E21)),SUM(E19,E20,E21),""))</f>
         <v/>
       </c>
-      <c r="F18" s="0" t="str">
+      <c r="F18" s="0" t="e">
         <f aca="false">IF(OR(,ISTEXT(A38),ISTEXT(A50)),SUM(F38,F50),IF(OR(ISNUMBER(F19),ISNUMBER(F20),ISNUMBER(F21)),SUM(F19,F20,F21),""))</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>30</v>
@@ -1213,12 +1234,12 @@
         <f aca="false">IF(OR(ISTEXT(G38),ISTEXT(G50)),SUM(K38,K50),IF(OR(ISNUMBER(K19),ISNUMBER(K20),ISNUMBER(K21)),SUM(K19,K20,K21),""))</f>
         <v/>
       </c>
-      <c r="L18" s="0" t="str">
+      <c r="L18" s="0" t="e">
         <f aca="false">IF(OR(,ISTEXT(G38),ISTEXT(G50)),SUM(L38,L50),IF(OR(ISNUMBER(L19),ISNUMBER(L20),ISNUMBER(L21)),SUM(L19,L20,L21),""))</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
         <v>31</v>
       </c>
@@ -1250,71 +1271,95 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="0" t="str">
+      <c r="D20" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
-        <v/>
-      </c>
-      <c r="E20" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E40),ISNUMBER(E52)),SUM(E40,E52),"")</f>
-        <v/>
-      </c>
-      <c r="F20" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F40),ISNUMBER(F52)),SUM(F40,F52),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I20" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="0" t="str">
+      <c r="J20" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(J40),ISNUMBER(J52)),SUM(J40,J52),"")</f>
-        <v/>
-      </c>
-      <c r="K20" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K20" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(K40),ISNUMBER(K52)),SUM(K40,K52),"")</f>
-        <v/>
-      </c>
-      <c r="L20" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L20" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(L40),ISNUMBER(L52)),SUM(L40,L52),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="0" t="str">
+      <c r="D21" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
-        <v/>
-      </c>
-      <c r="E21" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E41),ISNUMBER(E53)),SUM(E41,E53),"")</f>
-        <v/>
-      </c>
-      <c r="F21" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F41),ISNUMBER(F53)),SUM(F41,F53),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I21" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="J21" s="0" t="str">
+      <c r="J21" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(J41),ISNUMBER(J53)),SUM(J41,J53),"")</f>
-        <v/>
-      </c>
-      <c r="K21" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K21" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(K41),ISNUMBER(K53)),SUM(K41,K53),"")</f>
-        <v/>
-      </c>
-      <c r="L21" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L21" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(L41),ISNUMBER(L53)),SUM(L41,L53),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>34</v>
       </c>
@@ -1334,7 +1379,7 @@
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
         <v>35</v>
       </c>
@@ -1366,71 +1411,95 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="0" t="str">
+      <c r="D24" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
-        <v/>
-      </c>
-      <c r="E24" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E24" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E28),ISNUMBER(E32)),SUM(E28,E32),"")</f>
-        <v/>
-      </c>
-      <c r="F24" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F28),ISNUMBER(F32)),SUM(F28,F32),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I24" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="J24" s="0" t="str">
+      <c r="J24" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(J28),ISNUMBER(J32)),SUM(J28,J32),"")</f>
-        <v/>
-      </c>
-      <c r="K24" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K24" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(K28),ISNUMBER(K32)),SUM(K28,K32),"")</f>
-        <v/>
-      </c>
-      <c r="L24" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L24" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(L28),ISNUMBER(L32)),SUM(L28,L32),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="0" t="str">
+      <c r="D25" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
-        <v/>
-      </c>
-      <c r="E25" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E25" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E29),ISNUMBER(E33)),SUM(E29,E33),"")</f>
-        <v/>
-      </c>
-      <c r="F25" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F29),ISNUMBER(F33)),SUM(F29,F33),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I25" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="0" t="str">
+      <c r="J25" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(J29),ISNUMBER(J33)),SUM(J29,J33),"")</f>
-        <v/>
-      </c>
-      <c r="K25" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K25" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(K29),ISNUMBER(K33)),SUM(K29,K33),"")</f>
-        <v/>
-      </c>
-      <c r="L25" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L25" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(L29),ISNUMBER(L33)),SUM(L29,L33),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>38</v>
       </c>
@@ -1462,7 +1531,7 @@
         <v>55</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
         <v>40</v>
       </c>
@@ -1470,7 +1539,7 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
         <v>41</v>
       </c>
@@ -1478,7 +1547,7 @@
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
         <v>42</v>
       </c>
@@ -1486,7 +1555,7 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>43</v>
       </c>
@@ -1503,7 +1572,7 @@
         <v>8</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I30" s="0" t="s">
         <v>44</v>
@@ -1518,9 +1587,9 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -1535,7 +1604,7 @@
         <v/>
       </c>
       <c r="I31" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J35),ISNUMBER(J39)),SUM(J35,J39),"")</f>
@@ -1550,73 +1619,97 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="0" t="str">
+        <v>47</v>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
-        <v/>
-      </c>
-      <c r="E32" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E32" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E36),ISNUMBER(E40)),SUM(E36,E40),"")</f>
-        <v/>
-      </c>
-      <c r="F32" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F32" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F36),ISNUMBER(F40)),SUM(F36,F40),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I32" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J32" s="0" t="str">
+        <v>47</v>
+      </c>
+      <c r="J32" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(J36),ISNUMBER(J40)),SUM(J36,J40),"")</f>
-        <v/>
-      </c>
-      <c r="K32" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K32" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(K36),ISNUMBER(K40)),SUM(K36,K40),"")</f>
-        <v/>
-      </c>
-      <c r="L32" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L32" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(L36),ISNUMBER(L40)),SUM(L36,L40),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="0" t="str">
+        <v>48</v>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
-        <v/>
-      </c>
-      <c r="E33" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E33" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E37),ISNUMBER(E41)),SUM(E37,E41),"")</f>
-        <v/>
-      </c>
-      <c r="F33" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F33" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F37),ISNUMBER(F41)),SUM(F37,F41),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I33" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="J33" s="0" t="str">
+        <v>48</v>
+      </c>
+      <c r="J33" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(J37),ISNUMBER(J41)),SUM(J37,J41),"")</f>
-        <v/>
-      </c>
-      <c r="K33" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K33" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(K37),ISNUMBER(K41)),SUM(K37,K41),"")</f>
-        <v/>
-      </c>
-      <c r="L33" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L33" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(L37),ISNUMBER(L41)),SUM(L37,L41),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -1631,7 +1724,7 @@
         <v/>
       </c>
       <c r="I34" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G35),ISTEXT(G36),ISTEXT(G37)),SUM(J35,J36,J37),"")</f>
@@ -1646,33 +1739,33 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -1687,7 +1780,7 @@
         <v/>
       </c>
       <c r="I38" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G39),ISTEXT(G40),ISTEXT(G41)),SUM(J39,J40,J41),"")</f>
@@ -1702,33 +1795,33 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -1743,7 +1836,7 @@
         <v/>
       </c>
       <c r="I42" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J43),ISNUMBER(J44),ISNUMBER(J45),ISNUMBER(J46),ISNUMBER(J47),ISNUMBER(J48),ISNUMBER(J49),ISNUMBER(J50),ISNUMBER(J51),ISNUMBER(J52),ISNUMBER(J53)),SUMIF(G43:G53,"&gt;""",J43:J53),"")</f>
@@ -1758,9 +1851,9 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -1775,7 +1868,7 @@
         <v/>
       </c>
       <c r="I43" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J47),ISNUMBER(J51)),SUM(J47,J51),"")</f>
@@ -1790,65 +1883,85 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D44" s="0" t="str">
+        <v>59</v>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
-        <v/>
-      </c>
-      <c r="E44" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E44" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E48),ISNUMBER(E52)),SUM(E48,E52),"")</f>
-        <v/>
-      </c>
-      <c r="F44" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F44" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F48),ISNUMBER(F52)),SUM(F48,F52),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="H44" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="J44" s="0" t="str">
+        <v>59</v>
+      </c>
+      <c r="J44" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(J48),ISNUMBER(J52)),SUM(J48,J52),"")</f>
-        <v/>
-      </c>
-      <c r="K44" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K44" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(K48),ISNUMBER(K52)),SUM(K48,K52),"")</f>
-        <v/>
-      </c>
-      <c r="L44" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L44" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(L48),ISNUMBER(L52)),SUM(L48,L52),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="0" t="str">
+        <v>60</v>
+      </c>
+      <c r="E45" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
-        <v/>
-      </c>
-      <c r="F45" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F45" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F49),ISNUMBER(F53)),SUM(F49,F53),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I45" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="K45" s="0" t="str">
+        <v>60</v>
+      </c>
+      <c r="K45" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(K49),ISNUMBER(K53)),SUM(K49,K53),"")</f>
-        <v/>
-      </c>
-      <c r="L45" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L45" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(L49),ISNUMBER(L53)),SUM(L49,L53),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -1863,7 +1976,7 @@
         <v/>
       </c>
       <c r="I46" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G47),ISTEXT(G48),ISTEXT(G49)),SUM(J47,J48,J49),"")</f>
@@ -1878,33 +1991,33 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -1919,7 +2032,7 @@
         <v/>
       </c>
       <c r="I50" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G51),ISTEXT(G52),ISTEXT(G53)),SUM(J51,J52,J53),"")</f>
@@ -1934,33 +2047,33 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -1975,7 +2088,7 @@
         <v/>
       </c>
       <c r="I54" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J55),ISNUMBER(J56)),SUM(J55,J56),"")</f>
@@ -1990,25 +2103,25 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -2023,7 +2136,7 @@
         <v/>
       </c>
       <c r="I57" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J58),ISNUMBER(J59)),SUM(J58,J59),"")</f>
@@ -2038,25 +2151,25 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C58" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -2071,7 +2184,7 @@
         <v>9.8</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J60" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J61),ISNUMBER(J62),ISNUMBER(J63),ISNUMBER(J64),ISNUMBER(J65),ISNUMBER(J66),ISNUMBER(J67)),SUM(J61:J67),"")</f>
@@ -2086,12 +2199,12 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -2103,31 +2216,31 @@
         <v>7</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -2139,36 +2252,36 @@
         <v>2.8</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -2183,7 +2296,7 @@
         <v/>
       </c>
       <c r="I68" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J69),ISNUMBER(J70)),SUM(J69,J70),"")</f>
@@ -2198,25 +2311,25 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -2231,7 +2344,7 @@
         <v>0.1</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J72),ISNUMBER(J73),ISNUMBER(J74),ISNUMBER(J75)),SUM(J72:J75),"")</f>
@@ -2246,25 +2359,25 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -2276,7 +2389,7 @@
         <v>0.1</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J74" s="0" t="n">
         <v>5</v>
@@ -2288,17 +2401,17 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C75" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -2310,10 +2423,10 @@
         <v>0.1</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="77">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
         <v>13</v>
       </c>
@@ -2345,12 +2458,12 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
+    <row r="81" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G81" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
+    <row r="83" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D83" s="0" t="n">
         <f aca="false">0.3+0.4</f>
@@ -2361,14 +2474,14 @@
         <v>0.9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
+    <row r="84" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D85" s="0" t="n">
         <f aca="false">D71+J71+D95</f>
@@ -2383,9 +2496,9 @@
         <v>6.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
+    <row r="86" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D86" s="0" t="n">
         <f aca="false">D74+D71</f>
@@ -2400,9 +2513,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
+    <row r="87" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D87" s="0" t="n">
         <f aca="false">IF(ISTEXT(A61), SUM(D71:D74),12345)</f>
@@ -2413,45 +2526,45 @@
         <v>0.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
+    <row r="89" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D89" s="0" t="n">
         <f aca="false">D86+D71</f>
         <v>25.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
+    <row r="90" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="91">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D91" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E91" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D92" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E92" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="F91" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
-      <c r="D92" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
-      <c r="D93" s="0" t="b">
+    </row>
+    <row r="93" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D93" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E93" s="0" t="b">
+      <c r="E93" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2460,24 +2573,24 @@
         <v>No</v>
       </c>
       <c r="J93" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K93" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D94" s="0" t="n">
         <f aca="false">D60+D61</f>
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
+    <row r="95" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D95" s="0" t="n">
         <f aca="false">D61+D62</f>
@@ -2491,7 +2604,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2506,8 +2619,8 @@
   </sheetPr>
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I3" activeCellId="0" pane="topLeft" sqref="I3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2521,9 +2634,9 @@
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.6887755102041"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
@@ -2532,16 +2645,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
@@ -2549,7 +2662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="0" t="n">
         <v>1997</v>
       </c>
@@ -2557,12 +2670,12 @@
         <v>1998</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>11</v>
@@ -2577,7 +2690,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>11</v>
@@ -2589,9 +2702,9 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -2606,9 +2719,9 @@
         <v>6.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -2623,15 +2736,15 @@
         <v>4.3</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -2643,23 +2756,23 @@
         <v>4.3</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -2671,20 +2784,20 @@
         <v>2.3</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
@@ -2699,9 +2812,9 @@
         <v>141.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
@@ -2716,12 +2829,12 @@
         <v>133.2</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -2736,15 +2849,15 @@
         <v/>
       </c>
       <c r="I13" s="0" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -2759,12 +2872,12 @@
         <v>66.6</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -2779,52 +2892,62 @@
         <v/>
       </c>
       <c r="I15" s="0" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
         <v>2</v>
       </c>
-      <c r="E16" s="0" t="str">
+      <c r="E16" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E28),ISNUMBER(E36),ISNUMBER(E48)),SUM(E28,E36,E48),"")</f>
-        <v/>
-      </c>
-      <c r="F16" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F28),ISNUMBER(F36),ISNUMBER(F48)),SUM(F28,F36,F48),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I16" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="0" t="str">
+        <v>125</v>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D37),ISNUMBER(D49)),SUM(D29,D37,D49),"")</f>
-        <v/>
-      </c>
-      <c r="E17" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E29),ISNUMBER(E37),ISNUMBER(E49)),SUM(E29,E37,E49),"")</f>
-        <v/>
-      </c>
-      <c r="F17" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F29),ISNUMBER(F37),ISNUMBER(F49)),SUM(F29,F37,F49),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I17" s="0" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -2834,17 +2957,17 @@
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(E38,E50),IF(OR(ISNUMBER(E19),ISNUMBER(E20),ISNUMBER(E21)),SUM(E19,E20,E21),""))</f>
         <v/>
       </c>
-      <c r="F18" s="0" t="str">
+      <c r="F18" s="0" t="e">
         <f aca="false">IF(OR(,ISTEXT(A38),ISTEXT(A50)),SUM(F38,F50),IF(OR(ISNUMBER(F19),ISNUMBER(F20),ISNUMBER(F21)),SUM(F19,F20,F21),""))</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -2859,60 +2982,72 @@
         <v/>
       </c>
       <c r="I19" s="0" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" s="0" t="str">
+        <v>128</v>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
-        <v/>
-      </c>
-      <c r="E20" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E40),ISNUMBER(E52)),SUM(E40,E52),"")</f>
-        <v/>
-      </c>
-      <c r="F20" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F40),ISNUMBER(F52)),SUM(F40,F52),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I20" s="0" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="D21" s="0" t="str">
+        <v>129</v>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
-        <v/>
-      </c>
-      <c r="E21" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E41),ISNUMBER(E53)),SUM(E41,E53),"")</f>
-        <v/>
-      </c>
-      <c r="F21" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F41),ISNUMBER(F53)),SUM(F41,F53),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I21" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -2927,55 +3062,67 @@
         <v/>
       </c>
       <c r="I23" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D24" s="0" t="str">
+        <v>133</v>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
-        <v/>
-      </c>
-      <c r="E24" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E24" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E28),ISNUMBER(E32)),SUM(E28,E32),"")</f>
-        <v/>
-      </c>
-      <c r="F24" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F28),ISNUMBER(F32)),SUM(F28,F32),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I24" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D25" s="0" t="str">
+        <v>134</v>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
-        <v/>
-      </c>
-      <c r="E25" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E25" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E29),ISNUMBER(E33)),SUM(E29,E33),"")</f>
-        <v/>
-      </c>
-      <c r="F25" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F29),ISNUMBER(F33)),SUM(F29,F33),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I25" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -2987,39 +3134,39 @@
         <v>66.6</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -3031,12 +3178,12 @@
         <v>8</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -3051,52 +3198,64 @@
         <v/>
       </c>
       <c r="I31" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="D32" s="0" t="str">
+        <v>143</v>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
-        <v/>
-      </c>
-      <c r="E32" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E32" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E36),ISNUMBER(E40)),SUM(E36,E40),"")</f>
-        <v/>
-      </c>
-      <c r="F32" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F32" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F36),ISNUMBER(F40)),SUM(F36,F40),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I32" s="0" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" s="0" t="str">
+        <v>144</v>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
-        <v/>
-      </c>
-      <c r="E33" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E33" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E37),ISNUMBER(E41)),SUM(E37,E41),"")</f>
-        <v/>
-      </c>
-      <c r="F33" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F33" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F37),ISNUMBER(F41)),SUM(F37,F41),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I33" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -3111,36 +3270,36 @@
         <v/>
       </c>
       <c r="I34" s="0" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -3155,36 +3314,36 @@
         <v/>
       </c>
       <c r="I38" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D42" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -3199,12 +3358,12 @@
         <v/>
       </c>
       <c r="I42" s="0" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -3219,45 +3378,53 @@
         <v/>
       </c>
       <c r="I43" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D44" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
         <v>2</v>
       </c>
-      <c r="E44" s="0" t="str">
+      <c r="E44" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E48),ISNUMBER(E52)),SUM(E48,E52),"")</f>
-        <v/>
-      </c>
-      <c r="F44" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F44" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F48),ISNUMBER(F52)),SUM(F48,F52),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="E45" s="0" t="str">
+        <v>156</v>
+      </c>
+      <c r="E45" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
-        <v/>
-      </c>
-      <c r="F45" s="0" t="str">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F45" s="0" t="inlineStr">
         <f aca="false">IF(OR(ISNUMBER(F49),ISNUMBER(F53)),SUM(F49,F53),"")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="I45" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -3272,42 +3439,42 @@
         <v/>
       </c>
       <c r="I46" s="0" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J48" s="0" t="n">
         <v>0.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -3322,42 +3489,42 @@
         <v/>
       </c>
       <c r="I50" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J51" s="0" t="n">
         <v>0.3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J53" s="0" t="n">
         <v>0.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -3372,28 +3539,28 @@
         <v/>
       </c>
       <c r="I54" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -3408,28 +3575,28 @@
         <v/>
       </c>
       <c r="I57" s="0" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C58" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -3444,15 +3611,15 @@
         <v>9.8</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -3464,28 +3631,28 @@
         <v>7</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -3497,36 +3664,36 @@
         <v>2.8</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -3541,28 +3708,28 @@
         <v/>
       </c>
       <c r="I68" s="0" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -3577,28 +3744,28 @@
         <v>0.1</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -3610,20 +3777,20 @@
         <v>0.1</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C75" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -3635,10 +3802,10 @@
         <v>0.1</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="77">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
         <v>13</v>
       </c>
@@ -3670,69 +3837,69 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
+    <row r="88" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D88" s="2" t="n">
         <f aca="false">D48*$J103</f>
         <v>10.2</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J88" s="2" t="n">
         <f aca="false">J48*$CJ103</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
+    <row r="96" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D96" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J96" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="97">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E97" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K97" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F98" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L98" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D99" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K99" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L99" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>0.1</v>
@@ -3741,7 +3908,7 @@
         <v>0.25</v>
       </c>
       <c r="H100" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J100" s="0" t="n">
         <v>0.1</v>
@@ -3750,9 +3917,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
+    <row r="103" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H103" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J103" s="2" t="n">
         <f aca="false">(J51+J53)/J48+0.1</f>
@@ -3762,7 +3929,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>